<commit_message>
Some more data entry by Rachel, bless her.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Distraction_Assignment_RP.xlsx
+++ b/raw-data-prep/raw_data/Distraction_Assignment_RP.xlsx
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,6 +691,214 @@
       </c>
       <c r="B40">
         <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>421</v>
+      </c>
+      <c r="B41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>422</v>
+      </c>
+      <c r="B42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>423</v>
+      </c>
+      <c r="B43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>424</v>
+      </c>
+      <c r="B44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>425</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>426</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>427</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>428</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>429</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>430</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>431</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>432</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>433</v>
+      </c>
+      <c r="B53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>434</v>
+      </c>
+      <c r="B54">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>435</v>
+      </c>
+      <c r="B55">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>436</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>437</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>438</v>
+      </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>439</v>
+      </c>
+      <c r="B59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>440</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>441</v>
+      </c>
+      <c r="B61">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>442</v>
+      </c>
+      <c r="B62">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>443</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>444</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>445</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>446</v>
+      </c>
+      <c r="B66">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>